<commit_message>
feat(backend): added backend with excel, test push
</commit_message>
<xml_diff>
--- a/todo-app-main/todo.xlsx
+++ b/todo-app-main/todo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Software Works\Front End Mentor - Intermediate\todo-app-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9AE65E-6DAD-4E26-8F63-7CEA1BBFA4B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0642B40-F4DD-4B59-8105-E8F02B6EED5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>id</t>
   </si>
@@ -34,6 +34,15 @@
   </si>
   <si>
     <t>isCompleted</t>
+  </si>
+  <si>
+    <t>10 mins meditation</t>
+  </si>
+  <si>
+    <t>Read for 1hr</t>
+  </si>
+  <si>
+    <t>Jog around park 3x</t>
   </si>
 </sst>
 </file>
@@ -351,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -374,6 +383,39 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>